<commit_message>
Update IEI members Excel data
</commit_message>
<xml_diff>
--- a/iei_processed_members.xlsx
+++ b/iei_processed_members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\IEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C5BE61-987E-4B7D-BAC6-CEFC5687E088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4591C41B-2515-4C9F-B9BE-E8478C366BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
   <si>
     <t>membership_id</t>
   </si>
@@ -76,12 +76,6 @@
     <t>SE</t>
   </si>
   <si>
-    <t>7354278961</t>
-  </si>
-  <si>
-    <t>8961</t>
-  </si>
-  <si>
     <t>AM1423502</t>
   </si>
   <si>
@@ -97,12 +91,6 @@
     <t>TE</t>
   </si>
   <si>
-    <t>7281069046</t>
-  </si>
-  <si>
-    <t>9046</t>
-  </si>
-  <si>
     <t>ST1423503</t>
   </si>
   <si>
@@ -118,12 +106,6 @@
     <t>BE</t>
   </si>
   <si>
-    <t>9494438320</t>
-  </si>
-  <si>
-    <t>8320</t>
-  </si>
-  <si>
     <t>T-1423504</t>
   </si>
   <si>
@@ -134,12 +116,6 @@
   </si>
   <si>
     <t>MECH</t>
-  </si>
-  <si>
-    <t>8862544799</t>
-  </si>
-  <si>
-    <t>4799</t>
   </si>
   <si>
     <t>F-1423505</t>
@@ -730,7 +706,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>7354278961</v>
+        <v>9356949919</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -816,126 +792,126 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
+      <c r="G3">
+        <v>9356949919</v>
+      </c>
+      <c r="H3">
+        <v>9919</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>7977603065</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>7281069046</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
+      <c r="G4">
+        <v>7977603065</v>
+      </c>
+      <c r="H4">
+        <v>3065</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>8855987935</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>9494438320</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
+      <c r="G5">
+        <v>8855987935</v>
+      </c>
+      <c r="H5">
+        <v>7935</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>8862544799</v>
+        <v>9867100946</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
+      <c r="G6">
+        <v>9867100946</v>
+      </c>
+      <c r="H6">
+        <v>946</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>8012652909</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>8977086312</v>
@@ -947,21 +923,21 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>7388606223</v>
@@ -970,76 +946,76 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>8416133305</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>7618272786</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>8401895171</v>
@@ -1051,21 +1027,21 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>8700049692</v>
@@ -1077,125 +1053,125 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>9979682993</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D15">
         <v>8751350519</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>9941761270</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D17">
         <v>6493734491</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>8385600250</v>
@@ -1207,21 +1183,21 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D19">
         <v>9884228158</v>
@@ -1230,65 +1206,65 @@
         <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D20">
         <v>9999736436</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D21">
         <v>9026566902</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update IEI members Excel locally
</commit_message>
<xml_diff>
--- a/iei_processed_members.xlsx
+++ b/iei_processed_members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\IEI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C5BE61-987E-4B7D-BAC6-CEFC5687E088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4591C41B-2515-4C9F-B9BE-E8478C366BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
   <si>
     <t>membership_id</t>
   </si>
@@ -76,12 +76,6 @@
     <t>SE</t>
   </si>
   <si>
-    <t>7354278961</t>
-  </si>
-  <si>
-    <t>8961</t>
-  </si>
-  <si>
     <t>AM1423502</t>
   </si>
   <si>
@@ -97,12 +91,6 @@
     <t>TE</t>
   </si>
   <si>
-    <t>7281069046</t>
-  </si>
-  <si>
-    <t>9046</t>
-  </si>
-  <si>
     <t>ST1423503</t>
   </si>
   <si>
@@ -118,12 +106,6 @@
     <t>BE</t>
   </si>
   <si>
-    <t>9494438320</t>
-  </si>
-  <si>
-    <t>8320</t>
-  </si>
-  <si>
     <t>T-1423504</t>
   </si>
   <si>
@@ -134,12 +116,6 @@
   </si>
   <si>
     <t>MECH</t>
-  </si>
-  <si>
-    <t>8862544799</t>
-  </si>
-  <si>
-    <t>4799</t>
   </si>
   <si>
     <t>F-1423505</t>
@@ -730,7 +706,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>7354278961</v>
+        <v>9356949919</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -816,126 +792,126 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
+      <c r="G3">
+        <v>9356949919</v>
+      </c>
+      <c r="H3">
+        <v>9919</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4">
+        <v>7977603065</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>7281069046</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
+      <c r="G4">
+        <v>7977603065</v>
+      </c>
+      <c r="H4">
+        <v>3065</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>8855987935</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>9494438320</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
+      <c r="G5">
+        <v>8855987935</v>
+      </c>
+      <c r="H5">
+        <v>7935</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>8862544799</v>
+        <v>9867100946</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
+      <c r="G6">
+        <v>9867100946</v>
+      </c>
+      <c r="H6">
+        <v>946</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>8012652909</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>8977086312</v>
@@ -947,21 +923,21 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>7388606223</v>
@@ -970,76 +946,76 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>8416133305</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>7618272786</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>8401895171</v>
@@ -1051,21 +1027,21 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>8700049692</v>
@@ -1077,125 +1053,125 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>9979682993</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D15">
         <v>8751350519</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D16">
         <v>9941761270</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D17">
         <v>6493734491</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>8385600250</v>
@@ -1207,21 +1183,21 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D19">
         <v>9884228158</v>
@@ -1230,65 +1206,65 @@
         <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D20">
         <v>9999736436</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D21">
         <v>9026566902</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>